<commit_message>
update 3(2)xlsx and new cope 3(2)xlsx
</commit_message>
<xml_diff>
--- a/3 (2).xlsx
+++ b/3 (2).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladf\OneDrive\Рабочий стол\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53B1D27-EDC0-4764-A67C-0726B0A1BCE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +35,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -45,15 +57,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +431,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>